<commit_message>
Bug fix and updated to show pictures in output as well.
</commit_message>
<xml_diff>
--- a/codestructure.xlsx
+++ b/codestructure.xlsx
@@ -36,15 +36,9 @@
     <t xml:space="preserve">  'stream': prepOutput,</t>
   </si>
   <si>
-    <t xml:space="preserve">  'pyout': prepPyOut,</t>
-  </si>
-  <si>
     <t xml:space="preserve">  'display_data': processDisplayOutput,</t>
   </si>
   <si>
-    <t xml:space="preserve">  'pyerr': prepPyErr,</t>
-  </si>
-  <si>
     <t xml:space="preserve">  'svg': prepNotYet,</t>
   </si>
   <si>
@@ -118,6 +112,12 @@
   </si>
   <si>
     <t>clean up LaTeX code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'pyout/execute_result': prepExecuteResult,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'pyerr/error': prepPyErr,</t>
   </si>
 </sst>
 </file>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -494,48 +494,48 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
@@ -589,112 +589,112 @@
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H37" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H41" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="5:8" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H43" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="5:8" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>